<commit_message>
Use BigInteger and BigDecimal
</commit_message>
<xml_diff>
--- a/src/test/resources/teda/LOAD_TEST.xlsx
+++ b/src/test/resources/teda/LOAD_TEST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pad\Projects\teda\src\test\resources\teda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pad\Projects\teda-framework\src\test\resources\teda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE3B3F5-A504-405E-807F-7FED8FC67B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64DD24C-6A06-4C8B-8199-029C06292176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cockpit" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>#Teda</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>STUDENT_OUT</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>NAME</t>
@@ -100,8 +97,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.000000000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -140,15 +138,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -199,7 +199,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13578" displayName="Table13578" ref="C4:F8" totalsRowShown="0">
   <autoFilter ref="C4:F8" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="#ID" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NAME" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="AGE"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="AVERAGE"/>
@@ -547,7 +547,7 @@
   </sheetPr>
   <dimension ref="B3:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -587,7 +587,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -619,7 +619,7 @@
   <dimension ref="B3:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,24 +635,24 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
@@ -660,7 +660,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>22</v>
@@ -674,7 +674,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>45</v>
@@ -688,7 +688,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>21</v>
@@ -702,12 +702,12 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>66</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="7">
         <v>4.3939494940000001</v>
       </c>
     </row>
@@ -773,41 +773,39 @@
   </sheetPr>
   <dimension ref="B3:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="21.453125" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="21.453125" customWidth="1"/>
-    <col min="6" max="6" width="29.1796875" customWidth="1"/>
+    <col min="3" max="3" width="26.36328125" customWidth="1"/>
+    <col min="4" max="4" width="32.54296875" customWidth="1"/>
+    <col min="5" max="5" width="29.81640625" customWidth="1"/>
+    <col min="6" max="6" width="36.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
@@ -815,12 +813,12 @@
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>22</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>12.66</v>
       </c>
     </row>
@@ -829,12 +827,12 @@
         <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>45</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>34.44</v>
       </c>
     </row>
@@ -843,12 +841,12 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>21</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>24.33</v>
       </c>
     </row>
@@ -857,12 +855,12 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>66</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <v>4.3939494940000001</v>
       </c>
     </row>
@@ -872,9 +870,6 @@
       <c r="F9" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C3:E3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>